<commit_message>
completed authentication in front-end with reset password function
</commit_message>
<xml_diff>
--- a/LG/DB.xlsx
+++ b/LG/DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Skillsync\LG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
   <si>
     <t>1.</t>
   </si>
@@ -50,9 +50,6 @@
     <t>number</t>
   </si>
   <si>
-    <t>char[50]</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>Teammates</t>
   </si>
   <si>
-    <t>ranking of each user in LoL game.</t>
-  </si>
-  <si>
     <t>ranking of each teammates in LoL game</t>
   </si>
   <si>
@@ -117,6 +111,78 @@
   </si>
   <si>
     <t>CustomersIDs</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>ranking in LoL game</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>display name in the site</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>ShortBio</t>
+  </si>
+  <si>
+    <t>Displayed in teammate selector</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reflect teammate's online status</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>PrimaryLang</t>
+  </si>
+  <si>
+    <t>Primaray language</t>
+  </si>
+  <si>
+    <t>SecondaryLang</t>
+  </si>
+  <si>
+    <t>Secondary language</t>
+  </si>
+  <si>
+    <t>DiscordUsername</t>
+  </si>
+  <si>
+    <t>Avartar</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>TeammateID</t>
+  </si>
+  <si>
+    <t>string[100]</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>reflect status of the order like waiting, accepted, cancled, finished</t>
+  </si>
+  <si>
+    <t>GameMode</t>
   </si>
 </sst>
 </file>
@@ -189,7 +255,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +285,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -571,196 +643,281 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,418 +1198,770 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O33"/>
+  <dimension ref="B1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.90625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" style="12" customWidth="1"/>
-    <col min="6" max="7" width="13.7265625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="21" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="12"/>
-    <col min="11" max="11" width="16.1796875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" style="12" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="12"/>
+    <col min="1" max="1" width="4.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" style="2"/>
+    <col min="14" max="14" width="14.6328125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="2:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="2:15" ht="16" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+      <c r="I4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="53"/>
+      <c r="C6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="2:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="38"/>
+      <c r="J7" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B8" s="45"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="36"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B9" s="45"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B10" s="45"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="36"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B11" s="45"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="12" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="46"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="37"/>
+    </row>
+    <row r="13" spans="2:18" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B14" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="2:18" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C16" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="O16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R16" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+    <row r="17" spans="2:18" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C17" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="R17" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B18" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="22"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B19" s="53"/>
+      <c r="C19" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="26"/>
+    </row>
+    <row r="20" spans="2:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="35"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B21" s="45"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="36"/>
+    </row>
+    <row r="22" spans="2:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="45"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="36"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B23" s="45"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="36"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B24" s="45"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="36"/>
+    </row>
+    <row r="25" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="46"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="37"/>
+    </row>
+    <row r="26" spans="2:18" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="2:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="2:18" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B30" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="H30" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B31" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="C31" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="27" t="s">
+      <c r="E31" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B32" s="53"/>
+      <c r="C32" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="45"/>
-      <c r="C6" s="28" t="s">
+      <c r="E32" s="76"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="26"/>
+    </row>
+    <row r="33" spans="2:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="2:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="39"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="47"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="40"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="47"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="47"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="47"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="40"/>
-    </row>
-    <row r="12" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="48"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="2:15" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="21"/>
-    </row>
-    <row r="15" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="21"/>
-    </row>
-    <row r="16" spans="2:15" ht="16" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="45"/>
-      <c r="C19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="17"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="47"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="40"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="47"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="40"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="47"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="40"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="47"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="40"/>
-    </row>
-    <row r="25" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="48"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="41"/>
-    </row>
-    <row r="26" spans="2:9" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="2:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="33" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="45"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="36"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="45"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="36"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="45"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="36"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="45"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="36"/>
+    </row>
+    <row r="38" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="46"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="37"/>
+    </row>
+    <row r="39" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="42">
+    <mergeCell ref="H33:H38"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C33:C38"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="H7:H12"/>
+    <mergeCell ref="K7:K12"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="F7:F12"/>
-    <mergeCell ref="G7:G12"/>
+    <mergeCell ref="I7:I12"/>
+    <mergeCell ref="J7:J12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="C20:C25"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="E20:E25"/>
+    <mergeCell ref="H20:H25"/>
+    <mergeCell ref="G7:G12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="H7:H12"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="I20:I25"/>
     <mergeCell ref="F20:F25"/>
-    <mergeCell ref="I20:I25"/>
+    <mergeCell ref="R20:R25"/>
+    <mergeCell ref="P20:P25"/>
     <mergeCell ref="G20:G25"/>
-    <mergeCell ref="H20:H25"/>
+    <mergeCell ref="K20:K25"/>
+    <mergeCell ref="L20:L25"/>
+    <mergeCell ref="M20:M25"/>
+    <mergeCell ref="O20:O25"/>
+    <mergeCell ref="J20:J25"/>
+    <mergeCell ref="N20:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>